<commit_message>
made some minor changes to the form automation. address string needed to be trimmed.
</commit_message>
<xml_diff>
--- a/UserRegistration/Excels/customer.xlsx
+++ b/UserRegistration/Excels/customer.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\tovar-practice\uipath\UserRegistration\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\Axel-Tovar-Automation_Challenge1\UserRegistration\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBE41AE-DD96-4117-B159-9C1E111B66C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C373FD3D-9498-42C5-98C1-DD1E42D05BBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{3C268B1C-FD3C-4C8E-B8D1-DF5DA02DDB04}"/>
   </bookViews>
@@ -68,49 +68,49 @@
     <t>Success</t>
   </si>
   <si>
-    <t>Richard</t>
-  </si>
-  <si>
-    <t>P.</t>
-  </si>
-  <si>
-    <t>RichardPThornton@teleworm.us</t>
-  </si>
-  <si>
-    <t>1394 Timbercrest RoadTatalina A.F.S., AK 99506</t>
-  </si>
-  <si>
-    <t>907-728-6619</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>S.</t>
-  </si>
-  <si>
-    <t>JamesSLine@dayrep.com</t>
-  </si>
-  <si>
-    <t>2589 Reppert Coal RoadSouthfield, MI 48075</t>
-  </si>
-  <si>
-    <t>586-890-9109</t>
-  </si>
-  <si>
-    <t>Myra</t>
-  </si>
-  <si>
-    <t>L.</t>
-  </si>
-  <si>
-    <t>MyraLAllen@dayrep.com</t>
-  </si>
-  <si>
-    <t>555 Raintree BoulevardIndianapolis, IN 46202</t>
-  </si>
-  <si>
-    <t>765-237-3200</t>
+    <t>Maureen</t>
+  </si>
+  <si>
+    <t>J.</t>
+  </si>
+  <si>
+    <t>MaureenJDelafuente@jourrapide.com</t>
+  </si>
+  <si>
+    <t>971 Alpha AvenueMarshall, TX 75670</t>
+  </si>
+  <si>
+    <t>903-938-1180</t>
+  </si>
+  <si>
+    <t>Arlene</t>
+  </si>
+  <si>
+    <t>K.</t>
+  </si>
+  <si>
+    <t>ArleneKSimon@jourrapide.com</t>
+  </si>
+  <si>
+    <t>4214 Reynolds AlleyBellflower, CA 90706</t>
+  </si>
+  <si>
+    <t>562-285-4192</t>
+  </si>
+  <si>
+    <t>Judy</t>
+  </si>
+  <si>
+    <t>D.</t>
+  </si>
+  <si>
+    <t>JudyDAllen@jourrapide.com</t>
+  </si>
+  <si>
+    <t>1403 Half and Half DriveKennedy Meadows, CA 93527</t>
+  </si>
+  <si>
+    <t>559-850-7665</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -536,7 +536,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -565,7 +565,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>

</xml_diff>